<commit_message>
Main changes here are adding some fifa ratings data to the model from fifaindex. I also added extra seasons worth of data and removed some of the XG data as that wasn't available for a lot of the earlier seasons.
</commit_message>
<xml_diff>
--- a/data/raw/team_name_lookup.xlsx
+++ b/data/raw/team_name_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reubenseager/Data Science Projects/2023/Betting Model/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49C3A99-B1E4-C146-8F3B-441779E27F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF84D97-EC57-AD48-89C5-D4952A7BFA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14440" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{CC50FD5D-9E7C-5941-8202-CC25F0DB63B3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{CC50FD5D-9E7C-5941-8202-CC25F0DB63B3}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="86">
   <si>
     <t>correct name</t>
   </si>
@@ -305,13 +305,25 @@
   </si>
   <si>
     <t>Sheffield Utd</t>
+  </si>
+  <si>
+    <t>Brighton &amp; Hove Albion</t>
+  </si>
+  <si>
+    <t>AFC Bournemouth</t>
+  </si>
+  <si>
+    <t>Bolton Wanderers</t>
+  </si>
+  <si>
+    <t>Wigan Athletic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,6 +337,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF657B83"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -347,9 +365,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CD2807-3238-A542-847B-E524BA911147}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1315,7 +1334,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>62</v>
       </c>
@@ -1331,7 +1350,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>63</v>
       </c>
@@ -1339,7 +1358,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>64</v>
       </c>
@@ -1347,7 +1366,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>37</v>
       </c>
@@ -1355,7 +1374,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>65</v>
       </c>
@@ -1363,7 +1382,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>66</v>
       </c>
@@ -1371,15 +1390,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>67</v>
       </c>
       <c r="B88" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G88" s="2"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>68</v>
       </c>
@@ -1387,7 +1407,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>69</v>
       </c>
@@ -1395,7 +1415,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -1403,7 +1423,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -1411,7 +1431,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -1419,7 +1439,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>53</v>
       </c>
@@ -1427,7 +1447,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>74</v>
       </c>
@@ -1435,7 +1455,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>75</v>
       </c>
@@ -1481,6 +1501,38 @@
       </c>
       <c r="B101" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>82</v>
+      </c>
+      <c r="B102" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>83</v>
+      </c>
+      <c r="B103" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>84</v>
+      </c>
+      <c r="B104" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>85</v>
+      </c>
+      <c r="B105" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>